<commit_message>
made changes to makejsons for some of the values to be coerced into integers from strings
</commit_message>
<xml_diff>
--- a/updated_script/Codebook for graphtext update.xlsx
+++ b/updated_script/Codebook for graphtext update.xlsx
@@ -1,23 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10211"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\ENechamkin\Desktop\WIP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dwood/Box Sync/sites/ed-data/updated_script/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AC10505-A1ED-9A45-81A8-A8E68DAD44DC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="29070" windowHeight="8535"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -327,7 +334,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -689,23 +696,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="29.28515625" customWidth="1"/>
-    <col min="2" max="2" width="8.140625" customWidth="1"/>
+    <col min="1" max="1" width="29.33203125" customWidth="1"/>
+    <col min="2" max="2" width="8.1640625" customWidth="1"/>
     <col min="3" max="3" width="17" customWidth="1"/>
-    <col min="4" max="5" width="16.42578125" customWidth="1"/>
-    <col min="6" max="6" width="73.140625" style="1" customWidth="1"/>
+    <col min="4" max="5" width="16.5" customWidth="1"/>
+    <col min="6" max="6" width="73.1640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="1" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>37</v>
       </c>
@@ -725,7 +732,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
@@ -745,7 +752,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
@@ -765,7 +772,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
@@ -785,7 +792,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>3</v>
       </c>
@@ -805,7 +812,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>4</v>
       </c>
@@ -825,7 +832,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>5</v>
       </c>
@@ -845,7 +852,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>6</v>
       </c>
@@ -865,7 +872,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>7</v>
       </c>
@@ -885,7 +892,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>8</v>
       </c>
@@ -905,7 +912,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>9</v>
       </c>
@@ -925,7 +932,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
         <v>10</v>
       </c>
@@ -945,7 +952,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
         <v>11</v>
       </c>
@@ -965,7 +972,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
         <v>12</v>
       </c>
@@ -985,7 +992,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
         <v>13</v>
       </c>
@@ -1005,7 +1012,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="8" t="s">
         <v>14</v>
       </c>
@@ -1025,7 +1032,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="8" t="s">
         <v>15</v>
       </c>
@@ -1045,7 +1052,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="8" t="s">
         <v>16</v>
       </c>
@@ -1065,7 +1072,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="8" t="s">
         <v>17</v>
       </c>
@@ -1085,7 +1092,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="8" t="s">
         <v>18</v>
       </c>
@@ -1105,7 +1112,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="8" t="s">
         <v>19</v>
       </c>
@@ -1125,7 +1132,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="8" t="s">
         <v>20</v>
       </c>
@@ -1145,7 +1152,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="8" t="s">
         <v>21</v>
       </c>
@@ -1165,7 +1172,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="8" t="s">
         <v>22</v>
       </c>
@@ -1185,7 +1192,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="8" t="s">
         <v>23</v>
       </c>
@@ -1205,7 +1212,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="8" t="s">
         <v>24</v>
       </c>
@@ -1225,7 +1232,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A27" s="8" t="s">
         <v>25</v>
       </c>
@@ -1245,7 +1252,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A28" s="8" t="s">
         <v>26</v>
       </c>
@@ -1265,7 +1272,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="63" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A29" s="8" t="s">
         <v>27</v>
       </c>
@@ -1285,7 +1292,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="63" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A30" s="8" t="s">
         <v>28</v>
       </c>
@@ -1305,7 +1312,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="8" t="s">
         <v>29</v>
       </c>
@@ -1325,7 +1332,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="8" t="s">
         <v>30</v>
       </c>
@@ -1345,7 +1352,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="8" t="s">
         <v>31</v>
       </c>
@@ -1365,7 +1372,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="8" t="s">
         <v>32</v>
       </c>
@@ -1385,7 +1392,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="8" t="s">
         <v>89</v>
       </c>
@@ -1405,7 +1412,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" s="8" t="s">
         <v>33</v>
       </c>
@@ -1425,7 +1432,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" s="8" t="s">
         <v>34</v>
       </c>
@@ -1445,7 +1452,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A38" s="8" t="s">
         <v>35</v>
       </c>
@@ -1465,7 +1472,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="141.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" ht="119" x14ac:dyDescent="0.2">
       <c r="A39" s="8" t="s">
         <v>36</v>
       </c>

</xml_diff>

<commit_message>
add data and updated graphtext, etc
</commit_message>
<xml_diff>
--- a/updated_script/Codebook for graphtext update.xlsx
+++ b/updated_script/Codebook for graphtext update.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dwood/Box Sync/sites/ed-data/updated_script/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2076CEF-743C-FD44-A556-83CD10C59D01}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32AEA640-3D28-044B-B503-16FF69729A46}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1600" yWindow="460" windowWidth="25600" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -713,8 +713,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>

</xml_diff>